<commit_message>
Add detail fields for input Description (in progress-commit 5)
Updated sample data.
Init some parts of marker data.
Finished rendering popup in Normal mode.
Finished init layout of popup in Edit mode.
Updated rendering some parts of popup in Edit mode.
</commit_message>
<xml_diff>
--- a/docs/db_sample.xlsx
+++ b/docs/db_sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="popup_layout" sheetId="6" r:id="rId1"/>
@@ -891,36 +891,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <t>&lt;p class='item-desc'&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{var}</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/p&gt;</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>var: Category name or SubCategory name or Group name</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1456,12 +1426,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>title
-NUL: not show label
-def: {subgrp.name or grp.name}: {marker.name}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>NUL</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1483,6 +1447,40 @@
     <t>search_title
 NUL: not show
 def: =title</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>title
+NUL: not show label
+def: {subgrp.name or grp.name or marker.name}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;p class='item-desc'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{var}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/p&gt;</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1493,7 +1491,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1549,15 +1547,6 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -1633,7 +1622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1651,19 +1640,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1676,6 +1665,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1985,8 +1976,8 @@
   </sheetPr>
   <dimension ref="B1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2016,16 +2007,16 @@
         <v>135</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>177</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>160</v>
@@ -2034,7 +2025,7 @@
         <v>143</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>137</v>
@@ -2051,16 +2042,16 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H2" t="s">
         <v>165</v>
       </c>
       <c r="K2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="2:12">
@@ -2074,16 +2065,16 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G3" t="s">
         <v>151</v>
       </c>
       <c r="I3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="2:12">
@@ -2097,16 +2088,16 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G4" t="s">
         <v>152</v>
       </c>
       <c r="I4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="2:12">
@@ -2123,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G5" t="s">
         <v>142</v>
@@ -2135,7 +2126,7 @@
         <v>157</v>
       </c>
       <c r="K5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:12">
@@ -2152,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G6" t="s">
         <v>156</v>
@@ -2164,7 +2155,7 @@
         <v>158</v>
       </c>
       <c r="K6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:12">
@@ -2181,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G7" t="s">
         <v>148</v>
@@ -2193,7 +2184,7 @@
         <v>145</v>
       </c>
       <c r="K7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -2210,7 +2201,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G8" t="s">
         <v>162</v>
@@ -2222,7 +2213,7 @@
         <v>149</v>
       </c>
       <c r="K8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L8" t="s">
         <v>139</v>
@@ -2242,7 +2233,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G9" t="s">
         <v>150</v>
@@ -2254,7 +2245,7 @@
         <v>154</v>
       </c>
       <c r="K9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -2271,7 +2262,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G10" t="s">
         <v>153</v>
@@ -2283,7 +2274,7 @@
         <v>159</v>
       </c>
       <c r="K10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L10" t="s">
         <v>140</v>
@@ -2303,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G11" t="s">
         <v>167</v>
@@ -2315,27 +2306,27 @@
         <v>169</v>
       </c>
       <c r="K11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="19">
         <v>1</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>170</v>
+      <c r="F12" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>298</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" t="s">
@@ -2368,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="7" customFormat="1">
@@ -2431,7 +2422,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="7" customFormat="1">
@@ -2450,7 +2441,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -2461,7 +2452,7 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -2472,7 +2463,7 @@
         <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -2483,7 +2474,7 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
         <v>51</v>
@@ -2519,12 +2510,12 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="40.5">
       <c r="A2" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>54</v>
@@ -2533,39 +2524,39 @@
         <v>52</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="H2" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="16" t="s">
         <v>250</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -2573,10 +2564,10 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -2584,10 +2575,10 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -2595,10 +2586,10 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -2606,10 +2597,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -2617,10 +2608,10 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -2628,10 +2619,10 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -2639,10 +2630,10 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -2650,10 +2641,10 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2661,10 +2652,10 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -2672,10 +2663,10 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -2683,10 +2674,10 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -2694,10 +2685,10 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -2705,10 +2696,10 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -2716,10 +2707,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2727,10 +2718,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
@@ -2738,10 +2729,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -2749,10 +2740,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
@@ -2914,7 +2905,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B35" t="s">
         <v>99</v>
@@ -2925,7 +2916,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B36" t="s">
         <v>100</v>
@@ -2936,7 +2927,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B37" t="s">
         <v>101</v>
@@ -2947,7 +2938,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B38" t="s">
         <v>102</v>
@@ -2958,7 +2949,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B39" t="s">
         <v>103</v>
@@ -2969,7 +2960,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B40" t="s">
         <v>104</v>
@@ -2980,7 +2971,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B41" t="s">
         <v>105</v>
@@ -2991,7 +2982,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B42" t="s">
         <v>106</v>
@@ -3002,7 +2993,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B43" t="s">
         <v>107</v>
@@ -3013,7 +3004,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B44" t="s">
         <v>108</v>
@@ -3024,7 +3015,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B45" t="s">
         <v>109</v>
@@ -3035,7 +3026,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B46" t="s">
         <v>110</v>
@@ -3046,7 +3037,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B47" t="s">
         <v>111</v>
@@ -3057,7 +3048,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B48" t="s">
         <v>112</v>
@@ -3068,7 +3059,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B49" t="s">
         <v>113</v>
@@ -3079,7 +3070,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B50" t="s">
         <v>114</v>
@@ -3090,7 +3081,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B51" t="s">
         <v>115</v>
@@ -3101,7 +3092,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B52" t="s">
         <v>116</v>
@@ -3112,7 +3103,7 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B53" t="s">
         <v>117</v>
@@ -3179,7 +3170,7 @@
         <v>3</v>
       </c>
       <c r="K58" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -3289,7 +3280,7 @@
         <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1">
@@ -3303,121 +3294,121 @@
         <v>41</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>222</v>
-      </c>
       <c r="F2" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="H2" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="16" t="s">
         <v>250</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -3590,13 +3581,13 @@
         <v>118</v>
       </c>
       <c r="B54" t="s">
+        <v>238</v>
+      </c>
+      <c r="C54" t="s">
         <v>239</v>
       </c>
-      <c r="C54" t="s">
-        <v>240</v>
-      </c>
       <c r="K54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3604,13 +3595,13 @@
         <v>118</v>
       </c>
       <c r="B55" t="s">
+        <v>254</v>
+      </c>
+      <c r="C55" t="s">
         <v>255</v>
       </c>
-      <c r="C55" t="s">
+      <c r="K55" t="s">
         <v>256</v>
-      </c>
-      <c r="K55" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3618,16 +3609,16 @@
         <v>119</v>
       </c>
       <c r="B56" t="s">
+        <v>264</v>
+      </c>
+      <c r="C56" t="s">
+        <v>263</v>
+      </c>
+      <c r="K56" t="s">
         <v>265</v>
       </c>
-      <c r="C56" t="s">
-        <v>264</v>
-      </c>
-      <c r="K56" t="s">
+      <c r="L56" t="s">
         <v>266</v>
-      </c>
-      <c r="L56" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3635,16 +3626,16 @@
         <v>119</v>
       </c>
       <c r="B57" t="s">
+        <v>270</v>
+      </c>
+      <c r="C57" t="s">
+        <v>269</v>
+      </c>
+      <c r="K57" t="s">
+        <v>272</v>
+      </c>
+      <c r="L57" t="s">
         <v>271</v>
-      </c>
-      <c r="C57" t="s">
-        <v>270</v>
-      </c>
-      <c r="K57" t="s">
-        <v>273</v>
-      </c>
-      <c r="L57" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3652,13 +3643,13 @@
         <v>119</v>
       </c>
       <c r="B58" t="s">
+        <v>275</v>
+      </c>
+      <c r="C58" t="s">
+        <v>274</v>
+      </c>
+      <c r="L58" t="s">
         <v>276</v>
-      </c>
-      <c r="C58" t="s">
-        <v>275</v>
-      </c>
-      <c r="L58" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3666,13 +3657,13 @@
         <v>120</v>
       </c>
       <c r="B59" t="s">
+        <v>258</v>
+      </c>
+      <c r="C59" t="s">
+        <v>257</v>
+      </c>
+      <c r="K59" t="s">
         <v>259</v>
-      </c>
-      <c r="C59" t="s">
-        <v>258</v>
-      </c>
-      <c r="K59" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -3680,13 +3671,13 @@
         <v>120</v>
       </c>
       <c r="B60" t="s">
+        <v>260</v>
+      </c>
+      <c r="C60" t="s">
         <v>261</v>
       </c>
-      <c r="C60" t="s">
+      <c r="K60" t="s">
         <v>262</v>
-      </c>
-      <c r="K60" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3694,13 +3685,13 @@
         <v>121</v>
       </c>
       <c r="B61" t="s">
+        <v>282</v>
+      </c>
+      <c r="C61" t="s">
+        <v>281</v>
+      </c>
+      <c r="L61" t="s">
         <v>283</v>
-      </c>
-      <c r="C61" t="s">
-        <v>282</v>
-      </c>
-      <c r="L61" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3708,13 +3699,13 @@
         <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C62" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L62" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -3722,13 +3713,13 @@
         <v>121</v>
       </c>
       <c r="B63" t="s">
+        <v>286</v>
+      </c>
+      <c r="C63" t="s">
         <v>287</v>
       </c>
-      <c r="C63" t="s">
-        <v>288</v>
-      </c>
       <c r="L63" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3736,13 +3727,13 @@
         <v>121</v>
       </c>
       <c r="B64" t="s">
+        <v>288</v>
+      </c>
+      <c r="C64" t="s">
         <v>289</v>
       </c>
-      <c r="C64" t="s">
-        <v>290</v>
-      </c>
       <c r="L64" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -3752,13 +3743,13 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
+        <v>223</v>
+      </c>
+      <c r="B66" t="s">
         <v>224</v>
       </c>
-      <c r="B66" t="s">
-        <v>225</v>
-      </c>
       <c r="C66" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -3766,21 +3757,21 @@
         <v>124</v>
       </c>
       <c r="B67" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C67" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C68" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -3788,10 +3779,10 @@
         <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C69" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -3804,10 +3795,10 @@
         <v>127</v>
       </c>
       <c r="B71" t="s">
+        <v>233</v>
+      </c>
+      <c r="C71" t="s">
         <v>234</v>
-      </c>
-      <c r="C71" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -3831,8 +3822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3859,72 +3850,72 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="7" customFormat="1" ht="54">
       <c r="A2" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>183</v>
-      </c>
       <c r="D2" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L2" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="M2" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="N2" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="O2" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="P2" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>250</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -3938,13 +3929,13 @@
         <v>60.99</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -3952,171 +3943,171 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" t="s">
         <v>225</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" t="s">
         <v>226</v>
-      </c>
-      <c r="I4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="D5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E5" t="s">
+        <v>227</v>
+      </c>
+      <c r="I5" t="s">
         <v>228</v>
-      </c>
-      <c r="I5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="D6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" t="s">
         <v>231</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
         <v>232</v>
-      </c>
-      <c r="I6" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="D7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="D8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="D9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F9" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K9" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="D10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="D11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="D12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="D13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="D14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="D15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="D16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="4:17">
       <c r="D17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="4:17">
       <c r="D18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="4:17">
       <c r="D19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="4:17">
       <c r="D20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E20" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q20" t="s">
         <v>280</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -4138,13 +4129,13 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C2" s="17">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>